<commit_message>
This is my corrected project
</commit_message>
<xml_diff>
--- a/Manual testcase/PolicyBazaarManualTesting.xlsx
+++ b/Manual testcase/PolicyBazaarManualTesting.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2303843\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745789C9-CD30-4D25-8259-419CC53DB4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43429763-55CF-40CF-8C11-347FABFF3A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E38668E8-A9F4-4624-B3D6-2342084C79D4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{E38668E8-A9F4-4624-B3D6-2342084C79D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="90">
   <si>
     <t>Test_Case_ID</t>
   </si>
@@ -120,12 +122,6 @@
     <t>TC_07</t>
   </si>
   <si>
-    <t>Filter Plans and Sort By</t>
-  </si>
-  <si>
-    <t>Filter and Sort by the details</t>
-  </si>
-  <si>
     <t>TC_08</t>
   </si>
   <si>
@@ -186,9 +182,6 @@
     <t>To verify the functionality of the plans form</t>
   </si>
   <si>
-    <t>1.Locate the Frequent Flyer Plans under Plan Type and click on it.                                                                     2. Locate the number of days input field and click on it.                    3. Verify whether the number of days input filed is selected                                                             4. Click Apply Button.                                                                              5. Locate the Sort By dropdown and click on it.                                                                                    6. Locate the Low to High option and click on the Radio Button.   7. Verify whether the Low to High option is selected.</t>
-  </si>
-  <si>
     <t>Print company names</t>
   </si>
   <si>
@@ -199,16 +192,130 @@
   </si>
   <si>
     <t>The total number of companies should be printed.                                                                                       The name of each company should be printed.                   The price for each company should be printed.</t>
+  </si>
+  <si>
+    <t>Print names and prices of company</t>
+  </si>
+  <si>
+    <t>TC_09</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sort By</t>
+  </si>
+  <si>
+    <t>1. Locate the Sort By dropdown and click on it.                                                                                    2. Locate the Low to High option and click on the Radio Button.   3. Verify whether the Low to High option is selected.</t>
+  </si>
+  <si>
+    <t>The “Sort By” dropdown should be clicked and the options should be displayed.
+The “Low to High” option should be selected after clicking.</t>
   </si>
   <si>
     <t>The “Frequent Flyer Plans” radio button should be selected after clicking.
 The “Number of Days” input field should be selected after clicking.
-The “Apply” button should be clicked and the user should be redirected to the next page.
-The “Sort By” dropdown should be clicked and the options should be displayed.
-The “Low to High” option should be selected after clicking.</t>
-  </si>
-  <si>
-    <t>Print names and prices of company</t>
+The “Apply” button should be clicked and the user should be redirected to the next page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Locate the Frequent Flyer Plans under Plan Type and click on it.                                                                     2. Locate the number of days input field and click on it.                    3. Verify whether the number of days input filed is selected                                                             4. Click Apply Button.                                                                              </t>
+  </si>
+  <si>
+    <t>Filter Plans</t>
+  </si>
+  <si>
+    <t>Filter the details that are required</t>
+  </si>
+  <si>
+    <t>Sort by the details that are required</t>
+  </si>
+  <si>
+    <t>Test Case ID</t>
+  </si>
+  <si>
+    <t>Test Case Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description </t>
+  </si>
+  <si>
+    <t>Test Steps</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>TC_10</t>
+  </si>
+  <si>
+    <t>Select Insurance Product in policybazaar page.</t>
+  </si>
+  <si>
+    <t>To verify the Insurance product in policybazaar page</t>
+  </si>
+  <si>
+    <t>1. Navigate to policybazaar website.         2. Click on the Insurance Product dropdown menu.                                           </t>
+  </si>
+  <si>
+    <t>The user is navigated to the insurance product page.</t>
+  </si>
+  <si>
+    <t>TC_11</t>
+  </si>
+  <si>
+    <t>Select Car Insurance in policybazaar page.</t>
+  </si>
+  <si>
+    <t>To verify the navigation and functionality of the car insurance feature on the policy bazaar page.</t>
+  </si>
+  <si>
+    <t>1.Select "Car Insurance" from the dropdown menu.                                             2. Verify whether the page title is correct. 3. Locate and click "Click here" button.</t>
+  </si>
+  <si>
+    <t>The user is navigated to the car insurance page.</t>
+  </si>
+  <si>
+    <t>Select the required car details</t>
+  </si>
+  <si>
+    <t>To verify the car insurance process on the policy Bazaar website.</t>
+  </si>
+  <si>
+    <t>1. Check whetehr the text "Select City &amp; RTO" is available on that page.                   2. Select "Chennai" from the city dropdown box.                                               3. Verify whether "Chennai" is selected successfully.                                                     4. Select "TN-01" from the RTO list.                  
+5. Verify whether the RTO is selected successfully.                                                        6. Select "Maruthi" from the car brand list. 
+7. Select "Baleno" from the car model list.  
+8. Check the text "Select car fuel " is available.                                                         9. Select "Petrol" as the fuel type.            
+10. Verify whether the "Delta AMT" variant is displayed and select it.</t>
+  </si>
+  <si>
+    <t>The user should be able to select the city, RTO, car brand , car model, fuel type and car variant successfully.</t>
+  </si>
+  <si>
+    <t>Enter the details</t>
+  </si>
+  <si>
+    <t>To verify the input validation for the fields required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Locate the name input field and  enter the name.                                                        2. Enter and verify  whether an error message is displayed.                                    3. Locate the email input field and enter the email.                                                          4. Enter and verify whether an error message is displayed.                                      5. Locate the mobile number input field and enter the number.                                 6. Enter and verify whether an error message is displayed.                                          7. Click on "View Prices" button.   </t>
+  </si>
+  <si>
+    <t>The user should be identify the error messages that are dispalyed while entering the values.</t>
+  </si>
+  <si>
+    <t>TC_12</t>
+  </si>
+  <si>
+    <t>TC_13</t>
+  </si>
+  <si>
+    <t>Insurance Product page is selected</t>
+  </si>
+  <si>
+    <t>Car Insurance is Selected</t>
+  </si>
+  <si>
+    <t>Car Details is Entered</t>
+  </si>
+  <si>
+    <t>Getting Error message while clicking on View prices</t>
   </si>
 </sst>
 </file>
@@ -250,12 +357,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB12AFB-8393-45F1-ABFB-0EFF8C992774}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -610,13 +723,13 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="58" x14ac:dyDescent="0.35">
@@ -627,13 +740,13 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="116" x14ac:dyDescent="0.35">
@@ -644,13 +757,13 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="120" customHeight="1" x14ac:dyDescent="0.35">
@@ -658,16 +771,16 @@
         <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="87" x14ac:dyDescent="0.35">
@@ -675,13 +788,13 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>21</v>
@@ -695,53 +808,65 @@
         <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
       <c r="B8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="E10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C11" s="1"/>
@@ -762,7 +887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{630A55AC-17EC-48AD-8A76-5715A8E40DDF}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -786,7 +911,7 @@
     </row>
     <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -797,7 +922,7 @@
     </row>
     <row r="3" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
@@ -808,7 +933,7 @@
     </row>
     <row r="4" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -819,7 +944,7 @@
     </row>
     <row r="5" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>18</v>
@@ -850,12 +975,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -863,19 +988,25 @@
     </row>
     <row r="9" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+    <row r="10" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
@@ -884,6 +1015,201 @@
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE76C416-2F13-465C-BBF8-38783A84B2F9}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.36328125" customWidth="1"/>
+    <col min="2" max="2" width="22.81640625" customWidth="1"/>
+    <col min="3" max="3" width="33.81640625" customWidth="1"/>
+    <col min="4" max="4" width="35.1796875" customWidth="1"/>
+    <col min="5" max="5" width="32.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="247" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B612FB0F-4049-4A1E-8208-7BD77E0DDDF3}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.36328125" customWidth="1"/>
+    <col min="2" max="2" width="35.1796875" customWidth="1"/>
+    <col min="3" max="3" width="16.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>